<commit_message>
update excels for initial plots
</commit_message>
<xml_diff>
--- a/halp/notebook/data/halp_lstm.xlsx
+++ b/halp/notebook/data/halp_lstm.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopheraberger/Dropbox/Kunle NIPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jian/Data/research/halp_float/halp/halp/notebook/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="65780" yWindow="5820" windowWidth="28040" windowHeight="16540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -115,7 +121,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -228,88 +234,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>6.7957799999999997</c:v>
+                  <c:v>6.79578</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.153499999999994</c:v>
+                  <c:v>66.15349999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.223799999999997</c:v>
+                  <c:v>73.2238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.558000000000007</c:v>
+                  <c:v>76.55800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.965199999999996</c:v>
+                  <c:v>77.9652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.338099999999997</c:v>
+                  <c:v>79.3381</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80.274600000000007</c:v>
+                  <c:v>80.2746</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.323899999999995</c:v>
+                  <c:v>81.32389999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82.588899999999995</c:v>
+                  <c:v>82.5889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>83.584199999999996</c:v>
+                  <c:v>83.5842</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.604100000000003</c:v>
+                  <c:v>84.6041</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>85.942599999999999</c:v>
+                  <c:v>85.9426</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.085099999999997</c:v>
+                  <c:v>87.0851</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>88.144199999999998</c:v>
+                  <c:v>88.1442</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.046300000000002</c:v>
+                  <c:v>89.0463</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90.272099999999995</c:v>
+                  <c:v>90.27209999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>91.497900000000001</c:v>
+                  <c:v>91.4979</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>92.0471</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>92.463800000000006</c:v>
+                  <c:v>92.4638</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92.630499999999998</c:v>
+                  <c:v>92.6305</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>93.017899999999997</c:v>
+                  <c:v>93.0179</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>93.061999999999998</c:v>
+                  <c:v>93.062</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>93.184600000000003</c:v>
+                  <c:v>93.1846</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>92.738399999999999</c:v>
+                  <c:v>92.7384</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>92.792400000000001</c:v>
+                  <c:v>92.7924</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>92.9983</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>93.042400000000001</c:v>
+                  <c:v>93.0424</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>93.385599999999997</c:v>
+                  <c:v>93.3856</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>93.6798</c:v>
@@ -318,7 +324,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3549-2749-89E7-B010E54844EA}"/>
             </c:ext>
@@ -358,97 +364,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>82.000500000000002</c:v>
+                  <c:v>82.0005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.785200000000003</c:v>
+                  <c:v>83.7852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.952399999999997</c:v>
+                  <c:v>85.9524</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.766400000000004</c:v>
+                  <c:v>86.7664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.801199999999994</c:v>
+                  <c:v>88.8012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.482699999999994</c:v>
+                  <c:v>89.4827</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.865399999999994</c:v>
+                  <c:v>90.86539999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90.885000000000005</c:v>
+                  <c:v>90.88500000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>91.988200000000006</c:v>
+                  <c:v>91.9882</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.071600000000004</c:v>
+                  <c:v>92.0716</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92.233400000000003</c:v>
+                  <c:v>92.2334</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.311800000000005</c:v>
+                  <c:v>92.3118</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91.292000000000002</c:v>
+                  <c:v>91.292</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>92.066699999999997</c:v>
+                  <c:v>92.0667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.380200000000002</c:v>
+                  <c:v>91.3802</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90.566299999999998</c:v>
+                  <c:v>90.5663</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>92.037300000000002</c:v>
+                  <c:v>92.0373</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>91.708799999999997</c:v>
+                  <c:v>91.7088</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>91.649900000000002</c:v>
+                  <c:v>91.6499</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>91.478300000000004</c:v>
+                  <c:v>91.4783</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89.482699999999994</c:v>
+                  <c:v>89.4827</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>91.135099999999994</c:v>
+                  <c:v>91.13509999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>90.595699999999994</c:v>
+                  <c:v>90.5957</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>89.909300000000002</c:v>
+                  <c:v>89.9093</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>90.561400000000006</c:v>
+                  <c:v>90.5614</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>91.708799999999997</c:v>
+                  <c:v>91.7088</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>90.605500000000006</c:v>
+                  <c:v>90.60550000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>90.576099999999997</c:v>
+                  <c:v>90.5761</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>90.899699999999996</c:v>
+                  <c:v>90.8997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3549-2749-89E7-B010E54844EA}"/>
             </c:ext>
@@ -487,13 +493,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3549-2749-89E7-B010E54844EA}"/>
             </c:ext>
@@ -532,97 +538,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>83.260599999999997</c:v>
+                  <c:v>83.2606</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86.045599999999993</c:v>
+                  <c:v>86.0456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.600099999999998</c:v>
+                  <c:v>88.6001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.576099999999997</c:v>
+                  <c:v>90.5761</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.870599999999996</c:v>
+                  <c:v>91.8706</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91.738200000000006</c:v>
+                  <c:v>91.7382</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92.498199999999997</c:v>
+                  <c:v>92.4982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.468699999999998</c:v>
+                  <c:v>92.4687</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>92.601100000000002</c:v>
+                  <c:v>92.6011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.336399999999998</c:v>
+                  <c:v>92.3364</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92.488399999999999</c:v>
+                  <c:v>92.4884</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.199100000000001</c:v>
+                  <c:v>92.1991</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>92.743300000000005</c:v>
+                  <c:v>92.7433</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>92.503100000000003</c:v>
+                  <c:v>92.5031</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>92.968900000000005</c:v>
+                  <c:v>92.9689</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.939400000000006</c:v>
+                  <c:v>92.9394</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>93.228700000000003</c:v>
+                  <c:v>93.2287</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>92.885499999999993</c:v>
+                  <c:v>92.88549999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>92.944299999999998</c:v>
+                  <c:v>92.9443</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92.694299999999998</c:v>
+                  <c:v>92.6943</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>93.302300000000002</c:v>
+                  <c:v>93.3023</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>93.061999999999998</c:v>
+                  <c:v>93.062</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>93.738699999999994</c:v>
+                  <c:v>93.7387</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>93.341499999999996</c:v>
+                  <c:v>93.3415</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>93.718999999999994</c:v>
+                  <c:v>93.719</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>93.439599999999999</c:v>
+                  <c:v>93.4396</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>93.875900000000001</c:v>
+                  <c:v>93.8759</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>93.576899999999995</c:v>
+                  <c:v>93.57689999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>94.022999999999996</c:v>
+                  <c:v>94.023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3549-2749-89E7-B010E54844EA}"/>
             </c:ext>
@@ -637,11 +643,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1713629407"/>
-        <c:axId val="1713574863"/>
+        <c:axId val="488641376"/>
+        <c:axId val="492050160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1713629407"/>
+        <c:axId val="488641376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1713574863"/>
+        <c:crossAx val="492050160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -749,10 +755,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1713574863"/>
+        <c:axId val="492050160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="75"/>
+          <c:min val="75.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -861,10 +867,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1713629407"/>
-        <c:crossesAt val="1"/>
+        <c:crossAx val="488641376"/>
+        <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -880,10 +886,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.48583708632361916"/>
-          <c:y val="0.61632213932685631"/>
-          <c:w val="0.48166138826742599"/>
-          <c:h val="4.0263093604946162E-2"/>
+          <c:x val="0.485837086323619"/>
+          <c:y val="0.616322139326856"/>
+          <c:w val="0.481661388267426"/>
+          <c:h val="0.0402630936049462"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -953,7 +959,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -997,6 +1003,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1033,10 +1040,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1270665327907837"/>
-          <c:y val="0.18478541723839481"/>
-          <c:w val="0.85106827670031182"/>
-          <c:h val="0.65654408815520049"/>
+          <c:x val="0.127066532790784"/>
+          <c:y val="0.184785417238395"/>
+          <c:w val="0.851068276700312"/>
+          <c:h val="0.6565440881552"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1075,88 +1082,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>6.7957799999999997</c:v>
+                  <c:v>6.79578</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.153499999999994</c:v>
+                  <c:v>66.15349999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.223799999999997</c:v>
+                  <c:v>73.2238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.558000000000007</c:v>
+                  <c:v>76.55800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.965199999999996</c:v>
+                  <c:v>77.9652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.338099999999997</c:v>
+                  <c:v>79.3381</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80.274600000000007</c:v>
+                  <c:v>80.2746</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.323899999999995</c:v>
+                  <c:v>81.32389999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82.588899999999995</c:v>
+                  <c:v>82.5889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>83.584199999999996</c:v>
+                  <c:v>83.5842</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.604100000000003</c:v>
+                  <c:v>84.6041</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>85.942599999999999</c:v>
+                  <c:v>85.9426</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.085099999999997</c:v>
+                  <c:v>87.0851</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>88.144199999999998</c:v>
+                  <c:v>88.1442</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.046300000000002</c:v>
+                  <c:v>89.0463</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90.272099999999995</c:v>
+                  <c:v>90.27209999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>91.497900000000001</c:v>
+                  <c:v>91.4979</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>92.0471</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>92.463800000000006</c:v>
+                  <c:v>92.4638</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92.630499999999998</c:v>
+                  <c:v>92.6305</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>93.017899999999997</c:v>
+                  <c:v>93.0179</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>93.061999999999998</c:v>
+                  <c:v>93.062</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>93.184600000000003</c:v>
+                  <c:v>93.1846</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>92.738399999999999</c:v>
+                  <c:v>92.7384</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>92.792400000000001</c:v>
+                  <c:v>92.7924</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>92.9983</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>93.042400000000001</c:v>
+                  <c:v>93.0424</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>93.385599999999997</c:v>
+                  <c:v>93.3856</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>93.6798</c:v>
@@ -1165,7 +1172,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EBBC-5444-A561-422B3C0AB4DD}"/>
             </c:ext>
@@ -1204,97 +1211,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>82.000500000000002</c:v>
+                  <c:v>82.0005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.785200000000003</c:v>
+                  <c:v>83.7852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.952399999999997</c:v>
+                  <c:v>85.9524</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.766400000000004</c:v>
+                  <c:v>86.7664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.801199999999994</c:v>
+                  <c:v>88.8012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.482699999999994</c:v>
+                  <c:v>89.4827</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.865399999999994</c:v>
+                  <c:v>90.86539999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90.885000000000005</c:v>
+                  <c:v>90.88500000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>91.988200000000006</c:v>
+                  <c:v>91.9882</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.071600000000004</c:v>
+                  <c:v>92.0716</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92.233400000000003</c:v>
+                  <c:v>92.2334</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.311800000000005</c:v>
+                  <c:v>92.3118</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91.292000000000002</c:v>
+                  <c:v>91.292</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>92.066699999999997</c:v>
+                  <c:v>92.0667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.380200000000002</c:v>
+                  <c:v>91.3802</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90.566299999999998</c:v>
+                  <c:v>90.5663</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>92.037300000000002</c:v>
+                  <c:v>92.0373</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>91.708799999999997</c:v>
+                  <c:v>91.7088</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>91.649900000000002</c:v>
+                  <c:v>91.6499</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>91.478300000000004</c:v>
+                  <c:v>91.4783</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89.482699999999994</c:v>
+                  <c:v>89.4827</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>91.135099999999994</c:v>
+                  <c:v>91.13509999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>90.595699999999994</c:v>
+                  <c:v>90.5957</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>89.909300000000002</c:v>
+                  <c:v>89.9093</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>90.561400000000006</c:v>
+                  <c:v>90.5614</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>91.708799999999997</c:v>
+                  <c:v>91.7088</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>90.605500000000006</c:v>
+                  <c:v>90.60550000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>90.576099999999997</c:v>
+                  <c:v>90.5761</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>90.899699999999996</c:v>
+                  <c:v>90.8997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EBBC-5444-A561-422B3C0AB4DD}"/>
             </c:ext>
@@ -1334,97 +1341,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>83.260599999999997</c:v>
+                  <c:v>83.2606</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86.045599999999993</c:v>
+                  <c:v>86.0456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.600099999999998</c:v>
+                  <c:v>88.6001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.576099999999997</c:v>
+                  <c:v>90.5761</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.870599999999996</c:v>
+                  <c:v>91.8706</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91.738200000000006</c:v>
+                  <c:v>91.7382</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92.498199999999997</c:v>
+                  <c:v>92.4982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.468699999999998</c:v>
+                  <c:v>92.4687</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>92.601100000000002</c:v>
+                  <c:v>92.6011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.336399999999998</c:v>
+                  <c:v>92.3364</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92.488399999999999</c:v>
+                  <c:v>92.4884</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.199100000000001</c:v>
+                  <c:v>92.1991</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>92.743300000000005</c:v>
+                  <c:v>92.7433</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>92.503100000000003</c:v>
+                  <c:v>92.5031</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>92.968900000000005</c:v>
+                  <c:v>92.9689</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.939400000000006</c:v>
+                  <c:v>92.9394</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>93.228700000000003</c:v>
+                  <c:v>93.2287</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>92.885499999999993</c:v>
+                  <c:v>92.88549999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>92.944299999999998</c:v>
+                  <c:v>92.9443</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92.694299999999998</c:v>
+                  <c:v>92.6943</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>93.302300000000002</c:v>
+                  <c:v>93.3023</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>93.061999999999998</c:v>
+                  <c:v>93.062</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>93.738699999999994</c:v>
+                  <c:v>93.7387</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>93.341499999999996</c:v>
+                  <c:v>93.3415</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>93.718999999999994</c:v>
+                  <c:v>93.719</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>93.439599999999999</c:v>
+                  <c:v>93.4396</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>93.875900000000001</c:v>
+                  <c:v>93.8759</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>93.576899999999995</c:v>
+                  <c:v>93.57689999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>94.022999999999996</c:v>
+                  <c:v>94.023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EBBC-5444-A561-422B3C0AB4DD}"/>
             </c:ext>
@@ -1466,94 +1473,94 @@
                   <c:v>86.7517</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.369900000000001</c:v>
+                  <c:v>89.3699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.733000000000004</c:v>
+                  <c:v>90.733</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.591099999999997</c:v>
+                  <c:v>91.5911</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.174599999999998</c:v>
+                  <c:v>92.1746</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92.282399999999996</c:v>
+                  <c:v>92.2824</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92.537400000000005</c:v>
+                  <c:v>92.5374</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.615799999999993</c:v>
+                  <c:v>92.61579999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>92.650199999999998</c:v>
+                  <c:v>92.6502</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>92.6404</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92.664900000000003</c:v>
+                  <c:v>92.6649</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.709000000000003</c:v>
+                  <c:v>92.709</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>92.713899999999995</c:v>
+                  <c:v>92.7139</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>91.846000000000004</c:v>
+                  <c:v>91.846</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>92.468699999999998</c:v>
+                  <c:v>92.4687</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.861000000000004</c:v>
+                  <c:v>92.861</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>92.856099999999998</c:v>
+                  <c:v>92.8561</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>93.218900000000005</c:v>
+                  <c:v>93.2189</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>93.336600000000004</c:v>
+                  <c:v>93.3366</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>93.572000000000003</c:v>
+                  <c:v>93.572</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>93.625900000000001</c:v>
+                  <c:v>93.6259</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>93.714100000000002</c:v>
+                  <c:v>93.7141</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>93.694500000000005</c:v>
+                  <c:v>93.6945</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>93.728899999999996</c:v>
+                  <c:v>93.7289</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>93.733800000000002</c:v>
+                  <c:v>93.7338</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>93.684700000000007</c:v>
+                  <c:v>93.68470000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>92.213800000000006</c:v>
+                  <c:v>92.2138</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>93.522900000000007</c:v>
+                  <c:v>93.52290000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>93.655299999999997</c:v>
+                  <c:v>93.6553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1438-6F48-944E-3FD9FDD5E659}"/>
             </c:ext>
@@ -1592,82 +1599,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>87.943100000000001</c:v>
+                  <c:v>87.9431</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.105699999999999</c:v>
+                  <c:v>91.1057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.316699999999997</c:v>
+                  <c:v>92.3167</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.022800000000004</c:v>
+                  <c:v>93.0228</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.547399999999996</c:v>
+                  <c:v>93.5474</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>94.076999999999998</c:v>
+                  <c:v>94.077</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>94.1113</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93.978899999999996</c:v>
+                  <c:v>93.9789</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>94.204499999999996</c:v>
+                  <c:v>94.2045</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>93.768100000000004</c:v>
+                  <c:v>93.7681</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>93.356200000000001</c:v>
+                  <c:v>93.3562</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>93.831800000000001</c:v>
+                  <c:v>93.8318</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>94.219200000000001</c:v>
+                  <c:v>94.2192</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>94.179900000000004</c:v>
+                  <c:v>94.1799</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>94.219200000000001</c:v>
+                  <c:v>94.2192</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>94.184799999999996</c:v>
+                  <c:v>94.1848</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>93.508200000000002</c:v>
+                  <c:v>93.5082</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>93.851399999999998</c:v>
+                  <c:v>93.8514</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.268199999999993</c:v>
+                  <c:v>94.2682</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>93.395399999999995</c:v>
+                  <c:v>93.3954</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>93.846500000000006</c:v>
+                  <c:v>93.8465</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>94.400599999999997</c:v>
+                  <c:v>94.4006</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>94.513400000000004</c:v>
+                  <c:v>94.5134</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>94.228999999999999</c:v>
+                  <c:v>94.229</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>94.150499999999994</c:v>
+                  <c:v>94.15049999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>93.444500000000005</c:v>
+                  <c:v>93.4445</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>93.9495</c:v>
@@ -1676,13 +1683,13 @@
                   <c:v>94.1554</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>94.253500000000003</c:v>
+                  <c:v>94.2535</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1438-6F48-944E-3FD9FDD5E659}"/>
             </c:ext>
@@ -1697,11 +1704,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1762599199"/>
-        <c:axId val="1762874175"/>
+        <c:axId val="466795856"/>
+        <c:axId val="517778688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1762599199"/>
+        <c:axId val="466795856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1733,6 +1740,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1799,7 +1807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1762874175"/>
+        <c:crossAx val="517778688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1809,10 +1817,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1762874175"/>
+        <c:axId val="517778688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="75"/>
+          <c:min val="75.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1861,6 +1869,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1921,10 +1930,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1762599199"/>
+        <c:crossAx val="466795856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1940,10 +1949,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.56067121609798776"/>
-          <c:y val="0.44397949093572608"/>
-          <c:w val="0.4393287839020123"/>
-          <c:h val="0.37634792162607583"/>
+          <c:x val="0.560671216097988"/>
+          <c:y val="0.443979490935726"/>
+          <c:w val="0.439328783902012"/>
+          <c:h val="0.376347921626076"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2013,7 +2022,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2057,6 +2066,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2128,307 +2138,307 @@
                   <c:v>2.4996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1041000000000001</c:v>
+                  <c:v>1.1041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91344800000000004</c:v>
+                  <c:v>0.913448</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.822079</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76873199999999997</c:v>
+                  <c:v>0.768732</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72276799999999997</c:v>
+                  <c:v>0.722768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.68205899999999997</c:v>
+                  <c:v>0.682059</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64322500000000005</c:v>
+                  <c:v>0.643225</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60419400000000001</c:v>
+                  <c:v>0.604194</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.58163500000000001</c:v>
+                  <c:v>0.581635</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.54473000000000005</c:v>
+                  <c:v>0.54473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.50212400000000001</c:v>
+                  <c:v>0.502124</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.47320099999999998</c:v>
+                  <c:v>0.473201</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43211500000000003</c:v>
+                  <c:v>0.432115</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.40292600000000001</c:v>
+                  <c:v>0.402926</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.36760799999999999</c:v>
+                  <c:v>0.367608</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.335032</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.31241999999999998</c:v>
+                  <c:v>0.31242</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29356199999999999</c:v>
+                  <c:v>0.293562</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.29216900000000001</c:v>
+                  <c:v>0.292169</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28257599999999999</c:v>
+                  <c:v>0.282576</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.28469899999999998</c:v>
+                  <c:v>0.284699</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.28853600000000001</c:v>
+                  <c:v>0.288536</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.31620900000000002</c:v>
+                  <c:v>0.316209</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.29998799999999998</c:v>
+                  <c:v>0.299988</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.29358400000000001</c:v>
+                  <c:v>0.293584</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.28835899999999998</c:v>
+                  <c:v>0.288359</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.27752100000000002</c:v>
+                  <c:v>0.277521</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.26835900000000001</c:v>
+                  <c:v>0.268359</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.26824599999999998</c:v>
+                  <c:v>0.268246</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.26569799999999999</c:v>
+                  <c:v>0.265698</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.27064700000000003</c:v>
+                  <c:v>0.270647</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0.273233</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.26960000000000001</c:v>
+                  <c:v>0.2696</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.26142700000000002</c:v>
+                  <c:v>0.261427</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.25641799999999998</c:v>
+                  <c:v>0.256418</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.25413799999999998</c:v>
+                  <c:v>0.254138</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.25668800000000003</c:v>
+                  <c:v>0.256688</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0.256191</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.25711600000000001</c:v>
+                  <c:v>0.257116</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.25601299999999999</c:v>
+                  <c:v>0.256013</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.25570799999999999</c:v>
+                  <c:v>0.255708</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.25559100000000001</c:v>
+                  <c:v>0.255591</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.25724999999999998</c:v>
+                  <c:v>0.25725</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.26187100000000002</c:v>
+                  <c:v>0.261871</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.26421499999999998</c:v>
+                  <c:v>0.264215</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.25894499999999998</c:v>
+                  <c:v>0.258945</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.25842900000000002</c:v>
+                  <c:v>0.258429</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.25956299999999999</c:v>
+                  <c:v>0.259563</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.25488899999999998</c:v>
+                  <c:v>0.254889</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.25732699999999997</c:v>
+                  <c:v>0.257327</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.25692399999999999</c:v>
+                  <c:v>0.256924</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.26208399999999998</c:v>
+                  <c:v>0.262084</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>0.258967</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.25931300000000002</c:v>
+                  <c:v>0.259313</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.25879099999999999</c:v>
+                  <c:v>0.258791</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.25140099999999999</c:v>
+                  <c:v>0.251401</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.25081100000000001</c:v>
+                  <c:v>0.250811</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.25516100000000003</c:v>
+                  <c:v>0.255161</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.25329600000000002</c:v>
+                  <c:v>0.253296</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.26050099999999998</c:v>
+                  <c:v>0.260501</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>0.258797</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.26395000000000002</c:v>
+                  <c:v>0.26395</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.26088299999999998</c:v>
+                  <c:v>0.260883</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.25707999999999998</c:v>
+                  <c:v>0.25708</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.25518999999999997</c:v>
+                  <c:v>0.25519</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.25673400000000002</c:v>
+                  <c:v>0.256734</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.25561899999999999</c:v>
+                  <c:v>0.255619</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.26175199999999998</c:v>
+                  <c:v>0.261752</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.25876100000000002</c:v>
+                  <c:v>0.258761</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.25994800000000001</c:v>
+                  <c:v>0.259948</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.25670999999999999</c:v>
+                  <c:v>0.25671</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.25658999999999998</c:v>
+                  <c:v>0.25659</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.25648199999999999</c:v>
+                  <c:v>0.256482</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.25570799999999999</c:v>
+                  <c:v>0.255708</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.27068999999999999</c:v>
+                  <c:v>0.27069</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.26027400000000001</c:v>
+                  <c:v>0.260274</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.25708300000000001</c:v>
+                  <c:v>0.257083</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.25628400000000001</c:v>
+                  <c:v>0.256284</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.25912800000000002</c:v>
+                  <c:v>0.259128</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.26207000000000003</c:v>
+                  <c:v>0.26207</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.26155400000000001</c:v>
+                  <c:v>0.261554</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.26133899999999999</c:v>
+                  <c:v>0.261339</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.26193699999999998</c:v>
+                  <c:v>0.261937</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0.262459</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.26194000000000001</c:v>
+                  <c:v>0.26194</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.26258300000000001</c:v>
+                  <c:v>0.262583</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.26760899999999999</c:v>
+                  <c:v>0.267609</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.27371099999999998</c:v>
+                  <c:v>0.273711</c:v>
                 </c:pt>
                 <c:pt idx="89">
                   <c:v>0.27464</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.27215299999999998</c:v>
+                  <c:v>0.272153</c:v>
                 </c:pt>
                 <c:pt idx="91">
                   <c:v>0.263486</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.26069999999999999</c:v>
+                  <c:v>0.2607</c:v>
                 </c:pt>
                 <c:pt idx="93">
                   <c:v>0.258405</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.25673499999999999</c:v>
+                  <c:v>0.256735</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.25798100000000002</c:v>
+                  <c:v>0.257981</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.25620999999999999</c:v>
+                  <c:v>0.25621</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.25604900000000003</c:v>
+                  <c:v>0.256049</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.26055099999999998</c:v>
+                  <c:v>0.260551</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.25439600000000001</c:v>
+                  <c:v>0.254396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-08F5-FE41-BB5A-C17383830860}"/>
             </c:ext>
@@ -2467,127 +2477,127 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.62051900000000004</c:v>
+                  <c:v>0.620519</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54791900000000004</c:v>
+                  <c:v>0.547919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50365300000000002</c:v>
+                  <c:v>0.503653</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.453374</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.40118199999999998</c:v>
+                  <c:v>0.401182</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38444899999999999</c:v>
+                  <c:v>0.384449</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.35846699999999998</c:v>
+                  <c:v>0.358467</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.323208</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.31394699999999998</c:v>
+                  <c:v>0.313947</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.307703</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.29616399999999998</c:v>
+                  <c:v>0.296164</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.277868</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32836700000000002</c:v>
+                  <c:v>0.328367</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.31571900000000003</c:v>
+                  <c:v>0.315719</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33802399999999999</c:v>
+                  <c:v>0.338024</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.35465600000000003</c:v>
+                  <c:v>0.354656</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33751999999999999</c:v>
+                  <c:v>0.33752</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.38762999999999997</c:v>
+                  <c:v>0.38763</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.37677699999999997</c:v>
+                  <c:v>0.376777</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.38564100000000001</c:v>
+                  <c:v>0.385641</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.38446000000000002</c:v>
+                  <c:v>0.38446</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.35030499999999998</c:v>
+                  <c:v>0.350305</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.42152899999999999</c:v>
+                  <c:v>0.421529</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.43458200000000002</c:v>
+                  <c:v>0.434582</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.489255</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.36787199999999998</c:v>
+                  <c:v>0.367872</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.38006200000000001</c:v>
+                  <c:v>0.380062</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.41360799999999998</c:v>
+                  <c:v>0.413608</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.38030599999999998</c:v>
+                  <c:v>0.380306</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.37310500000000002</c:v>
+                  <c:v>0.373105</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.37373200000000001</c:v>
+                  <c:v>0.373732</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.45688299999999998</c:v>
+                  <c:v>0.456883</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.38781900000000002</c:v>
+                  <c:v>0.387819</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.37552200000000002</c:v>
+                  <c:v>0.375522</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.38183800000000001</c:v>
+                  <c:v>0.381838</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.36588199999999999</c:v>
+                  <c:v>0.365882</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0.317249</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.35649799999999998</c:v>
+                  <c:v>0.356498</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0.286833</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.27424700000000002</c:v>
+                  <c:v>0.274247</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.32433699999999999</c:v>
+                  <c:v>0.324337</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0.354354</c:v>
@@ -2596,181 +2606,181 @@
                   <c:v>0.344775</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.34959400000000002</c:v>
+                  <c:v>0.349594</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0.273974</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.29275800000000002</c:v>
+                  <c:v>0.292758</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.34566599999999997</c:v>
+                  <c:v>0.345666</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.33563100000000001</c:v>
+                  <c:v>0.335631</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.30115799999999998</c:v>
+                  <c:v>0.301158</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.34788599999999997</c:v>
+                  <c:v>0.347886</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>0.30462</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.35148299999999999</c:v>
+                  <c:v>0.351483</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.31802399999999997</c:v>
+                  <c:v>0.318024</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.39916600000000002</c:v>
+                  <c:v>0.399166</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>0.336808</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.29630499999999999</c:v>
+                  <c:v>0.296305</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.31154100000000001</c:v>
+                  <c:v>0.311541</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>0.339644</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.31613000000000002</c:v>
+                  <c:v>0.31613</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.34924300000000003</c:v>
+                  <c:v>0.349243</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.32303500000000002</c:v>
+                  <c:v>0.323035</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.34045500000000001</c:v>
+                  <c:v>0.340455</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.28254200000000002</c:v>
+                  <c:v>0.282542</c:v>
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>0.316191</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.31381300000000001</c:v>
+                  <c:v>0.313813</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.32785199999999998</c:v>
+                  <c:v>0.327852</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.31628899999999999</c:v>
+                  <c:v>0.316289</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.34651300000000002</c:v>
+                  <c:v>0.346513</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0.374913</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.35489799999999999</c:v>
+                  <c:v>0.354898</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.33030599999999999</c:v>
+                  <c:v>0.330306</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0.340258</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.34828100000000001</c:v>
+                  <c:v>0.348281</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.32564199999999999</c:v>
+                  <c:v>0.325642</c:v>
                 </c:pt>
                 <c:pt idx="74">
                   <c:v>0.369195</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.44967299999999999</c:v>
+                  <c:v>0.449673</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.42364800000000002</c:v>
+                  <c:v>0.423648</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.37981900000000002</c:v>
+                  <c:v>0.379819</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.33422400000000002</c:v>
+                  <c:v>0.334224</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.33019900000000002</c:v>
+                  <c:v>0.330199</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.38354899999999997</c:v>
+                  <c:v>0.383549</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.40194200000000002</c:v>
+                  <c:v>0.401942</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.41548400000000002</c:v>
+                  <c:v>0.415484</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.45751900000000001</c:v>
+                  <c:v>0.457519</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.39474999999999999</c:v>
+                  <c:v>0.39475</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.31485600000000002</c:v>
+                  <c:v>0.314856</c:v>
                 </c:pt>
                 <c:pt idx="86">
                   <c:v>0.381299</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.37193399999999999</c:v>
+                  <c:v>0.371934</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.37268099999999998</c:v>
+                  <c:v>0.372681</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.32365699999999997</c:v>
+                  <c:v>0.323657</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.34452899999999997</c:v>
+                  <c:v>0.344529</c:v>
                 </c:pt>
                 <c:pt idx="91">
                   <c:v>0.299178</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.32214900000000002</c:v>
+                  <c:v>0.322149</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.35470099999999999</c:v>
+                  <c:v>0.354701</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.34241899999999997</c:v>
+                  <c:v>0.342419</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.34322000000000003</c:v>
+                  <c:v>0.34322</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>0.337812</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.31078299999999998</c:v>
+                  <c:v>0.310783</c:v>
                 </c:pt>
                 <c:pt idx="98">
                   <c:v>0.325123</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.27383800000000003</c:v>
+                  <c:v>0.273838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-08F5-FE41-BB5A-C17383830860}"/>
             </c:ext>
@@ -2809,58 +2819,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.42008000000000001</c:v>
+                  <c:v>0.42008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31141799999999997</c:v>
+                  <c:v>0.311418</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.277252</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27038699999999999</c:v>
+                  <c:v>0.270387</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25253700000000001</c:v>
+                  <c:v>0.252537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23680100000000001</c:v>
+                  <c:v>0.236801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23192199999999999</c:v>
+                  <c:v>0.231922</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24770500000000001</c:v>
+                  <c:v>0.247705</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.214558</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.28042400000000001</c:v>
+                  <c:v>0.280424</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.29722700000000002</c:v>
+                  <c:v>0.297227</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.26718799999999998</c:v>
+                  <c:v>0.267188</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.22270300000000001</c:v>
+                  <c:v>0.222703</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.242283</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.22228800000000001</c:v>
+                  <c:v>0.222288</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.24021300000000001</c:v>
+                  <c:v>0.240213</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.28124300000000002</c:v>
+                  <c:v>0.281243</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.26261899999999999</c:v>
+                  <c:v>0.262619</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.234343</c:v>
@@ -2869,7 +2879,7 @@
                   <c:v>0.300367</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28485700000000003</c:v>
+                  <c:v>0.284857</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0.217088</c:v>
@@ -2878,106 +2888,106 @@
                   <c:v>0.208402</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.22187999999999999</c:v>
+                  <c:v>0.22188</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.24668100000000001</c:v>
+                  <c:v>0.246681</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.22725100000000001</c:v>
+                  <c:v>0.227251</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.24230099999999999</c:v>
+                  <c:v>0.242301</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.21366399999999999</c:v>
+                  <c:v>0.213664</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.23685400000000001</c:v>
+                  <c:v>0.236854</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.23307600000000001</c:v>
+                  <c:v>0.233076</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.22100900000000001</c:v>
+                  <c:v>0.221009</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.20597199999999999</c:v>
+                  <c:v>0.205972</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.21326700000000001</c:v>
+                  <c:v>0.213267</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.24313899999999999</c:v>
+                  <c:v>0.243139</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.29953800000000003</c:v>
+                  <c:v>0.299538</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.22387699999999999</c:v>
+                  <c:v>0.223877</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0.23093</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.34346700000000002</c:v>
+                  <c:v>0.343467</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.24514900000000001</c:v>
+                  <c:v>0.245149</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.22203700000000001</c:v>
+                  <c:v>0.222037</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.20683399999999999</c:v>
+                  <c:v>0.206834</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.24727099999999999</c:v>
+                  <c:v>0.247271</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.22476599999999999</c:v>
+                  <c:v>0.224766</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.25647500000000001</c:v>
+                  <c:v>0.256475</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0.2445</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.24593899999999999</c:v>
+                  <c:v>0.245939</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>0.234511</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.23528399999999999</c:v>
+                  <c:v>0.235284</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.22289400000000001</c:v>
+                  <c:v>0.222894</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.21885199999999999</c:v>
+                  <c:v>0.218852</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.23957899999999999</c:v>
+                  <c:v>0.239579</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.27039600000000003</c:v>
+                  <c:v>0.270396</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.23821000000000001</c:v>
+                  <c:v>0.23821</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.23729700000000001</c:v>
+                  <c:v>0.237297</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.35211300000000001</c:v>
+                  <c:v>0.352113</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.22451399999999999</c:v>
+                  <c:v>0.224514</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.22043299999999999</c:v>
+                  <c:v>0.220433</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>0.215307</c:v>
@@ -2989,7 +2999,7 @@
                   <c:v>0.22877</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.23541999999999999</c:v>
+                  <c:v>0.23542</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>0.229353</c:v>
@@ -2998,34 +3008,34 @@
                   <c:v>0.242504</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.24543200000000001</c:v>
+                  <c:v>0.245432</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.21268200000000001</c:v>
+                  <c:v>0.212682</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.21513699999999999</c:v>
+                  <c:v>0.215137</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.23318700000000001</c:v>
+                  <c:v>0.233187</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.23383699999999999</c:v>
+                  <c:v>0.233837</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.26842700000000003</c:v>
+                  <c:v>0.268427</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.25826300000000002</c:v>
+                  <c:v>0.258263</c:v>
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>0.220466</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.26329799999999998</c:v>
+                  <c:v>0.263298</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.25569999999999998</c:v>
+                  <c:v>0.2557</c:v>
                 </c:pt>
                 <c:pt idx="73">
                   <c:v>0.229684</c:v>
@@ -3043,13 +3053,13 @@
                   <c:v>0.236535</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.23561299999999999</c:v>
+                  <c:v>0.235613</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.27769100000000002</c:v>
+                  <c:v>0.277691</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.21052999999999999</c:v>
+                  <c:v>0.21053</c:v>
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>0.21653</c:v>
@@ -3058,61 +3068,61 @@
                   <c:v>0.213062</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.22711100000000001</c:v>
+                  <c:v>0.227111</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0.228768</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.25958100000000001</c:v>
+                  <c:v>0.259581</c:v>
                 </c:pt>
                 <c:pt idx="86">
                   <c:v>0.243029</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.26161000000000001</c:v>
+                  <c:v>0.26161</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.23452600000000001</c:v>
+                  <c:v>0.234526</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.28444199999999997</c:v>
+                  <c:v>0.284442</c:v>
                 </c:pt>
                 <c:pt idx="90">
                   <c:v>0.28197</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.20379900000000001</c:v>
+                  <c:v>0.203799</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>0.214113</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.23824999999999999</c:v>
+                  <c:v>0.23825</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.22339100000000001</c:v>
+                  <c:v>0.223391</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.25483699999999998</c:v>
+                  <c:v>0.254837</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.24484400000000001</c:v>
+                  <c:v>0.244844</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.25783499999999998</c:v>
+                  <c:v>0.257835</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.24293500000000001</c:v>
+                  <c:v>0.242935</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.25947300000000001</c:v>
+                  <c:v>0.259473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-08F5-FE41-BB5A-C17383830860}"/>
             </c:ext>
@@ -3151,16 +3161,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.61226599999999998</c:v>
+                  <c:v>0.612266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46753800000000001</c:v>
+                  <c:v>0.467538</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41795500000000002</c:v>
+                  <c:v>0.417955</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34381299999999998</c:v>
+                  <c:v>0.343813</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.330683</c:v>
@@ -3169,34 +3179,34 @@
                   <c:v>0.342941</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.34716599999999997</c:v>
+                  <c:v>0.347166</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.34245700000000001</c:v>
+                  <c:v>0.342457</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.34568900000000002</c:v>
+                  <c:v>0.345689</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35364899999999999</c:v>
+                  <c:v>0.353649</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35511799999999999</c:v>
+                  <c:v>0.355118</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.34797299999999998</c:v>
+                  <c:v>0.347973</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.348939</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.33560099999999998</c:v>
+                  <c:v>0.335601</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.32406800000000002</c:v>
+                  <c:v>0.324068</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.32476100000000002</c:v>
+                  <c:v>0.324761</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.32144</c:v>
@@ -3205,124 +3215,124 @@
                   <c:v>0.317969</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.32653500000000002</c:v>
+                  <c:v>0.326535</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.33335599999999999</c:v>
+                  <c:v>0.333356</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.33416800000000002</c:v>
+                  <c:v>0.334168</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.31182100000000001</c:v>
+                  <c:v>0.311821</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.32512799999999997</c:v>
+                  <c:v>0.325128</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.31112099999999998</c:v>
+                  <c:v>0.311121</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.33008500000000002</c:v>
+                  <c:v>0.330085</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.30125200000000002</c:v>
+                  <c:v>0.301252</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.30834099999999998</c:v>
+                  <c:v>0.308341</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.30603599999999997</c:v>
+                  <c:v>0.306036</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.29832599999999998</c:v>
+                  <c:v>0.298326</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.29342200000000002</c:v>
+                  <c:v>0.293422</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.30431799999999998</c:v>
+                  <c:v>0.304318</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.29016999999999998</c:v>
+                  <c:v>0.29017</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.30408400000000002</c:v>
+                  <c:v>0.304084</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.30305700000000002</c:v>
+                  <c:v>0.303057</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.31316100000000002</c:v>
+                  <c:v>0.313161</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.31886500000000001</c:v>
+                  <c:v>0.318865</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0.318913</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.28890300000000002</c:v>
+                  <c:v>0.288903</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.28031600000000001</c:v>
+                  <c:v>0.280316</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.30339300000000002</c:v>
+                  <c:v>0.303393</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.26604100000000003</c:v>
+                  <c:v>0.266041</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0.322274</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.29476000000000002</c:v>
+                  <c:v>0.29476</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.30384299999999997</c:v>
+                  <c:v>0.303843</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.29009000000000001</c:v>
+                  <c:v>0.29009</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.30399500000000002</c:v>
+                  <c:v>0.303995</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.30289300000000002</c:v>
+                  <c:v>0.302893</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.32967299999999999</c:v>
+                  <c:v>0.329673</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.28106399999999998</c:v>
+                  <c:v>0.281064</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.31577499999999997</c:v>
+                  <c:v>0.315775</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.31220799999999999</c:v>
+                  <c:v>0.312208</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.31036599999999998</c:v>
+                  <c:v>0.310366</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.29313899999999998</c:v>
+                  <c:v>0.293139</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.34489799999999998</c:v>
+                  <c:v>0.344898</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.24804300000000001</c:v>
+                  <c:v>0.248043</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.30220900000000001</c:v>
+                  <c:v>0.302209</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.25810499999999997</c:v>
+                  <c:v>0.258105</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.26127899999999998</c:v>
+                  <c:v>0.261279</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0.222859</c:v>
@@ -3331,7 +3341,7 @@
                   <c:v>0.251363</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.23174600000000001</c:v>
+                  <c:v>0.231746</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>0.244397</c:v>
@@ -3340,91 +3350,91 @@
                   <c:v>0.243173</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.25785200000000003</c:v>
+                  <c:v>0.257852</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.27189099999999999</c:v>
+                  <c:v>0.271891</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.26198199999999999</c:v>
+                  <c:v>0.261982</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>0.275565</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.30295899999999998</c:v>
+                  <c:v>0.302959</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0.269841</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.26000600000000001</c:v>
+                  <c:v>0.260006</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.29367100000000002</c:v>
+                  <c:v>0.293671</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.30201499999999998</c:v>
+                  <c:v>0.302015</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.24654499999999999</c:v>
+                  <c:v>0.246545</c:v>
                 </c:pt>
                 <c:pt idx="73">
                   <c:v>0.240899</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.26641700000000001</c:v>
+                  <c:v>0.266417</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.26369900000000002</c:v>
+                  <c:v>0.263699</c:v>
                 </c:pt>
                 <c:pt idx="76">
                   <c:v>0.256749</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.26509199999999999</c:v>
+                  <c:v>0.265092</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.27422400000000002</c:v>
+                  <c:v>0.274224</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.26630999999999999</c:v>
+                  <c:v>0.26631</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.27988299999999999</c:v>
+                  <c:v>0.279883</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.29604599999999998</c:v>
+                  <c:v>0.296046</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.29805199999999998</c:v>
+                  <c:v>0.298052</c:v>
                 </c:pt>
                 <c:pt idx="83">
                   <c:v>0.280223</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.27402300000000002</c:v>
+                  <c:v>0.274023</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.24700900000000001</c:v>
+                  <c:v>0.247009</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.26496399999999998</c:v>
+                  <c:v>0.264964</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.27563500000000002</c:v>
+                  <c:v>0.275635</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.29517399999999999</c:v>
+                  <c:v>0.295174</c:v>
                 </c:pt>
                 <c:pt idx="89">
                   <c:v>0.283854</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.27532000000000001</c:v>
+                  <c:v>0.27532</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.25799699999999998</c:v>
+                  <c:v>0.257997</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>0.23698</c:v>
@@ -3433,7 +3443,7 @@
                   <c:v>0.276391</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.26746999999999999</c:v>
+                  <c:v>0.26747</c:v>
                 </c:pt>
                 <c:pt idx="95">
                   <c:v>0.267955</c:v>
@@ -3442,10 +3452,10 @@
                   <c:v>0.250832</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.25192500000000001</c:v>
+                  <c:v>0.251925</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.24357799999999999</c:v>
+                  <c:v>0.243578</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0.243726</c:v>
@@ -3454,7 +3464,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-08F5-FE41-BB5A-C17383830860}"/>
             </c:ext>
@@ -3493,58 +3503,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.44916800000000001</c:v>
+                  <c:v>0.449168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37612400000000001</c:v>
+                  <c:v>0.376124</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.349744</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34753800000000001</c:v>
+                  <c:v>0.347538</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34400700000000001</c:v>
+                  <c:v>0.344007</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.351939</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.35692400000000002</c:v>
+                  <c:v>0.356924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35489599999999999</c:v>
+                  <c:v>0.354896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36142600000000003</c:v>
+                  <c:v>0.361426</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36056700000000003</c:v>
+                  <c:v>0.360567</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.36369400000000002</c:v>
+                  <c:v>0.363694</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.36244399999999999</c:v>
+                  <c:v>0.362444</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.36305900000000002</c:v>
+                  <c:v>0.363059</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.39791599999999999</c:v>
+                  <c:v>0.397916</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.35362100000000002</c:v>
+                  <c:v>0.353621</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.33778200000000003</c:v>
+                  <c:v>0.337782</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33085900000000001</c:v>
+                  <c:v>0.330859</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.32643699999999998</c:v>
+                  <c:v>0.326437</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.331397</c:v>
@@ -3553,151 +3563,151 @@
                   <c:v>0.320824</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.32211600000000001</c:v>
+                  <c:v>0.322116</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.32202399999999998</c:v>
+                  <c:v>0.322024</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.31658900000000001</c:v>
+                  <c:v>0.316589</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.31590499999999999</c:v>
+                  <c:v>0.315905</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.31539099999999998</c:v>
+                  <c:v>0.315391</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.31503199999999998</c:v>
+                  <c:v>0.315032</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.41999300000000001</c:v>
+                  <c:v>0.419993</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.30618899999999999</c:v>
+                  <c:v>0.306189</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.30397299999999999</c:v>
+                  <c:v>0.303973</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.31254300000000002</c:v>
+                  <c:v>0.312543</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.30589100000000002</c:v>
+                  <c:v>0.305891</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.31547399999999998</c:v>
+                  <c:v>0.315474</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0.305699</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.30622899999999997</c:v>
+                  <c:v>0.306229</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>0.307695</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.30414000000000002</c:v>
+                  <c:v>0.30414</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0.301371</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.29270699999999999</c:v>
+                  <c:v>0.292707</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.32856200000000002</c:v>
+                  <c:v>0.328562</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.28867900000000002</c:v>
+                  <c:v>0.288679</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.30961899999999998</c:v>
+                  <c:v>0.309619</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.31004399999999999</c:v>
+                  <c:v>0.310044</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0.294041</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.29322999999999999</c:v>
+                  <c:v>0.29323</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.29411799999999999</c:v>
+                  <c:v>0.294118</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.30108800000000002</c:v>
+                  <c:v>0.301088</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.27445199999999997</c:v>
+                  <c:v>0.274452</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0.278111</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.29928100000000002</c:v>
+                  <c:v>0.299281</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.29731600000000002</c:v>
+                  <c:v>0.297316</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.31334299999999998</c:v>
+                  <c:v>0.313343</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.28368500000000002</c:v>
+                  <c:v>0.283685</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.27073999999999998</c:v>
+                  <c:v>0.27074</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.26699000000000001</c:v>
+                  <c:v>0.26699</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.26375999999999999</c:v>
+                  <c:v>0.26376</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.27452599999999999</c:v>
+                  <c:v>0.274526</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.37663099999999999</c:v>
+                  <c:v>0.376631</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.26680300000000001</c:v>
+                  <c:v>0.266803</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.27060400000000001</c:v>
+                  <c:v>0.270604</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.26783000000000001</c:v>
+                  <c:v>0.26783</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.27831400000000001</c:v>
+                  <c:v>0.278314</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.29599799999999998</c:v>
+                  <c:v>0.295998</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.27222600000000002</c:v>
+                  <c:v>0.272226</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.27217000000000002</c:v>
+                  <c:v>0.27217</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.27037099999999997</c:v>
+                  <c:v>0.270371</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.26562799999999998</c:v>
+                  <c:v>0.265628</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.27837200000000001</c:v>
+                  <c:v>0.278372</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.31098900000000002</c:v>
+                  <c:v>0.310989</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.33083200000000001</c:v>
+                  <c:v>0.330832</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>0.314193</c:v>
@@ -3706,46 +3716,46 @@
                   <c:v>0.281887</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.28617100000000001</c:v>
+                  <c:v>0.286171</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.27696900000000002</c:v>
+                  <c:v>0.276969</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.27761200000000003</c:v>
+                  <c:v>0.277612</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.29339900000000002</c:v>
+                  <c:v>0.293399</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.28274500000000002</c:v>
+                  <c:v>0.282745</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.28962599999999999</c:v>
+                  <c:v>0.289626</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.28735100000000002</c:v>
+                  <c:v>0.287351</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.27379300000000001</c:v>
+                  <c:v>0.273793</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.28544700000000001</c:v>
+                  <c:v>0.285447</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.30099199999999998</c:v>
+                  <c:v>0.300992</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.26476899999999998</c:v>
+                  <c:v>0.264769</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.26907399999999998</c:v>
+                  <c:v>0.269074</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.28507399999999999</c:v>
+                  <c:v>0.285074</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.27974500000000002</c:v>
+                  <c:v>0.279745</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0.268762</c:v>
@@ -3754,40 +3764,40 @@
                   <c:v>0.24997</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.27116000000000001</c:v>
+                  <c:v>0.27116</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.27590300000000001</c:v>
+                  <c:v>0.275903</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.32237199999999999</c:v>
+                  <c:v>0.322372</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.28757500000000003</c:v>
+                  <c:v>0.287575</c:v>
                 </c:pt>
                 <c:pt idx="91">
                   <c:v>0.263797</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.27883799999999997</c:v>
+                  <c:v>0.278838</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.27311600000000003</c:v>
+                  <c:v>0.273116</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.27068199999999998</c:v>
+                  <c:v>0.270682</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.27007599999999998</c:v>
+                  <c:v>0.270076</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.28134199999999998</c:v>
+                  <c:v>0.281342</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.29718499999999998</c:v>
+                  <c:v>0.297185</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.27236500000000002</c:v>
+                  <c:v>0.272365</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0.301537</c:v>
@@ -3796,7 +3806,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-08F5-FE41-BB5A-C17383830860}"/>
             </c:ext>
@@ -3811,11 +3821,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="925166368"/>
-        <c:axId val="925168064"/>
+        <c:axId val="409952240"/>
+        <c:axId val="343787008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="925166368"/>
+        <c:axId val="409952240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3847,6 +3857,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3912,7 +3923,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="925168064"/>
+        <c:crossAx val="343787008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3921,7 +3932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="925168064"/>
+        <c:axId val="343787008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -3969,6 +3980,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4029,7 +4041,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="925166368"/>
+        <c:crossAx val="409952240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4047,10 +4059,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23406321550231754"/>
-          <c:y val="0.12775655625691418"/>
-          <c:w val="0.76591598257664606"/>
-          <c:h val="6.2326088371185008E-2"/>
+          <c:x val="0.234063215502318"/>
+          <c:y val="0.127756556256914"/>
+          <c:w val="0.765915982576646"/>
+          <c:h val="0.062326088371185"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4084,14 +4096,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5814,7 +5826,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5996B8B9-76AD-DF4D-AED7-BF8703D23CAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5996B8B9-76AD-DF4D-AED7-BF8703D23CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5835,13 +5847,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -5850,7 +5862,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7AE95F-3B6C-8840-9283-11963CE8DE6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B7AE95F-3B6C-8840-9283-11963CE8DE6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5875,23 +5887,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBB6645D-2A26-5B4C-8AA5-5F4CE6F74F26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DBB6645D-2A26-5B4C-8AA5-5F4CE6F74F26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6211,7 +6223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -13336,7 +13348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>

</xml_diff>